<commit_message>
UPDATE: Update intent template
</commit_message>
<xml_diff>
--- a/module/admin-api/InitFiles/intent_template.xlsx
+++ b/module/admin-api/InitFiles/intent_template.xlsx
@@ -5,14 +5,15 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielwu/workspaces/emotigo/module/admin-api/InitFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielwu/go-workspace/src/emotibot.com/emotigo/module/admin-api/InitFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="请在此页填写你的意图名称和positive语句" sheetId="1" r:id="rId1"/>
+    <sheet name="请在此页填写你的意图名称和negative语句" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="626">
   <si>
     <t>意图名称</t>
   </si>
@@ -2359,8 +2360,8 @@
   <sheetPr codeName="工作表1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B619"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7326,4 +7327,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="2" width="62.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>